<commit_message>
Added excel homework 14Feb2020
</commit_message>
<xml_diff>
--- a/bin/profile.xlsx
+++ b/bin/profile.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimke\OneDrive\Documents\investment and trading\stocks and equity\sandbox\WealthAndFreedom\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae26920bfc737752/Documents/investment and trading/stocks and equity/sandbox/WealthAndFreedom/bin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="114_{11E5F515-8949-44D0-953D-282568501902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8A6CAF08-CC40-4512-BCF7-C6D8BDF4DBC2}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="114_{11E5F515-8949-44D0-953D-282568501902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7BA5567D-1FC2-47B9-9C7D-F2F3451D6BA6}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11355" yWindow="0" windowWidth="17445" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="126">
   <si>
     <t>stockcode</t>
   </si>
@@ -211,6 +219,198 @@
   </si>
   <si>
     <t>BANK</t>
+  </si>
+  <si>
+    <t>FBMKLCI</t>
+  </si>
+  <si>
+    <t>大马富时合指数</t>
+  </si>
+  <si>
+    <t>大众银行</t>
+  </si>
+  <si>
+    <t>马来亚银行</t>
+  </si>
+  <si>
+    <t>联昌国际</t>
+  </si>
+  <si>
+    <t>丰隆银行</t>
+  </si>
+  <si>
+    <t>大马银行</t>
+  </si>
+  <si>
+    <t>兴业银行</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUNREIT </t>
+  </si>
+  <si>
+    <t>双威产托</t>
+  </si>
+  <si>
+    <t>INDICES</t>
+  </si>
+  <si>
+    <t>Consumer Products &amp; Services</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Financial Services</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Plantation</t>
+  </si>
+  <si>
+    <t>Real Estate Investment Trusts</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Telecommunications &amp; Media</t>
+  </si>
+  <si>
+    <t>Transportation and Logistics</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Structured Warrants</t>
+  </si>
+  <si>
+    <t>Exchange Traded Fund-Equity</t>
+  </si>
+  <si>
+    <t>Exchange Traded Fund-Commodity</t>
+  </si>
+  <si>
+    <t>Bond Islamic</t>
+  </si>
+  <si>
+    <t>Special Purpose Acquisition Company</t>
+  </si>
+  <si>
+    <t>Closed End Fund</t>
+  </si>
+  <si>
+    <t>Exchange Traded Fund-Bond</t>
+  </si>
+  <si>
+    <t>产托</t>
+  </si>
+  <si>
+    <t>Dow Jones Industrial Average</t>
+  </si>
+  <si>
+    <t>INDEXDJX: .DJI</t>
+  </si>
+  <si>
+    <t>S&amp;P 500 Index</t>
+  </si>
+  <si>
+    <t>INDEXSP: .INX</t>
+  </si>
+  <si>
+    <t>Nasdaq Composite</t>
+  </si>
+  <si>
+    <t>INDEXNASDAQ: .IXIC</t>
+  </si>
+  <si>
+    <t>美股道琼指数</t>
+  </si>
+  <si>
+    <t>标普 500 指数</t>
+  </si>
+  <si>
+    <t>那斯达克指数</t>
+  </si>
+  <si>
+    <t>来百利</t>
+  </si>
+  <si>
+    <t>大马顶级手套</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARTA </t>
+  </si>
+  <si>
+    <t>贺特佳</t>
+  </si>
+  <si>
+    <t>Hartalega Holdings Berhad</t>
+  </si>
+  <si>
+    <t>MBMR</t>
+  </si>
+  <si>
+    <t>MBM RESOURCES BHD</t>
+  </si>
+  <si>
+    <t>大马交易</t>
+  </si>
+  <si>
+    <t>BURSA</t>
+  </si>
+  <si>
+    <t>Bursa Malaysia Bhd</t>
+  </si>
+  <si>
+    <t>国油贸易</t>
+  </si>
+  <si>
+    <t>国油气体</t>
+  </si>
+  <si>
+    <t>国油化学</t>
+  </si>
+  <si>
+    <t>马国际船务</t>
+  </si>
+  <si>
+    <t>PETDAG</t>
+  </si>
+  <si>
+    <t>PETGAS</t>
+  </si>
+  <si>
+    <t>PCHEM</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t>Petronas Dagangan Berhad</t>
+  </si>
+  <si>
+    <t>Petronas Gas Bhd</t>
+  </si>
+  <si>
+    <t>PETRONAS CHEMICALS GROUP BHD</t>
+  </si>
+  <si>
+    <t>MISC Bhd</t>
+  </si>
+  <si>
+    <t>British American Tobacco (Mlys) Bhd</t>
+  </si>
+  <si>
+    <t>BAT</t>
   </si>
 </sst>
 </file>
@@ -264,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -282,31 +482,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -483,6 +667,25 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -518,21 +721,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60C0B303-7D27-4232-AAF3-B658FC4A76AA}" name="Table1" displayName="Table1" ref="A1:R16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:R16" xr:uid="{8BFEDBF4-44FA-48AF-B1AB-D58BEE1FC2CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60C0B303-7D27-4232-AAF3-B658FC4A76AA}" name="Table1" displayName="Table1" ref="A1:R49" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:R49" xr:uid="{8BFEDBF4-44FA-48AF-B1AB-D58BEE1FC2CE}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{72A8279B-C63E-49F8-9750-21200C4E832E}" name="stockcode" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{2BD30B7F-5CD4-4700-B50A-6403670360BD}" name="stockname" dataDxfId="9"/>
     <tableColumn id="12" xr3:uid="{21BC7494-A458-4527-9C74-387D451B8D2E}" name="name" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{F38F789C-7360-45FB-B5BD-C1D960CCF16C}" name="chinese" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{10E4968A-C8A8-4E79-88EA-DC8833B7DF7B}" name="notes" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{779C00A5-74D1-4654-B817-390112848D78}" name="board" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{11F99818-9EAC-4854-AE05-AE7AD3A8DD3F}" name="sector" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{D45AEAD6-5657-49C5-86E0-C0523BDBD08C}" name="industry" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{4030BC49-EF65-4C36-9CFF-F371B0E33F0E}" name="first trading date" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{10E4968A-C8A8-4E79-88EA-DC8833B7DF7B}" name="notes" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{779C00A5-74D1-4654-B817-390112848D78}" name="board" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{11F99818-9EAC-4854-AE05-AE7AD3A8DD3F}" name="sector" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{D45AEAD6-5657-49C5-86E0-C0523BDBD08C}" name="industry" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{4030BC49-EF65-4C36-9CFF-F371B0E33F0E}" name="first trading date" dataDxfId="2"/>
     <tableColumn id="15" xr3:uid="{7B3F8B5B-49E2-46C4-814C-76985C45132E}" name="company url"/>
-    <tableColumn id="3" xr3:uid="{920F15E2-4219-4E46-876F-9BBDF3844FF2}" name="klse" dataDxfId="2" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{CB34D860-F23D-4E09-9925-0D4875F13748}" name="klse charting" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{920F15E2-4219-4E46-876F-9BBDF3844FF2}" name="klse" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{CB34D860-F23D-4E09-9925-0D4875F13748}" name="klse charting" dataDxfId="0" dataCellStyle="Hyperlink"/>
     <tableColumn id="5" xr3:uid="{DD476CE4-D8D7-43A0-ACD6-2F2D4CF68D90}" name="bursa"/>
     <tableColumn id="7" xr3:uid="{A3885323-7D49-425F-A2FA-BD1A428FA45B}" name="trading view"/>
     <tableColumn id="19" xr3:uid="{BC341101-9657-4B8A-8377-8530144FB5E7}" name="i3investor"/>
@@ -807,17 +1010,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -893,304 +1097,742 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B23" s="2">
         <v>7803</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I23" s="5">
         <v>35536</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B24" s="2">
         <v>7106</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="I24" s="5"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B25" s="2">
         <v>7113</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="I25" s="5"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="2">
+        <v>5168</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B27" s="2">
         <v>7153</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="I27" s="5"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B28" s="2">
         <v>2127</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="I28" s="5"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="I29" s="5"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B30" s="2">
         <v>5185</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="I30" s="5"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B31" s="2">
         <v>1171</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="I31" s="5"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B32" s="2">
         <v>1155</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="I32" s="5"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B33" s="2">
         <v>1023</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="I33" s="5"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B34" s="2">
         <v>1295</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="I34" s="5"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B35" s="2">
         <v>1066</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="I35" s="5"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B36" s="2">
         <v>1015</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="I36" s="5"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B37" s="2">
         <v>5819</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="I37" s="5"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B38" s="2">
         <v>2488</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="I38" s="5"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="2">
+        <v>5176</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="2">
+        <v>5983</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1818</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="2">
+        <v>5681</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="2">
+        <v>6033</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="2">
+        <v>5183</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="2">
+        <v>3816</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" s="2">
+        <v>4162</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I49" s="5"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{7507FAC6-3C31-4D34-96D3-809B037A1804}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{4B2682E2-45B8-4BB8-ACD2-5E05F6C13CF9}"/>
-    <hyperlink ref="M2" r:id="rId3" xr:uid="{B4188B97-9CCE-4810-A77D-E94661EB9F84}"/>
-    <hyperlink ref="Q2" r:id="rId4" xr:uid="{1E7D945F-FEE7-4F42-9704-096D37B64E27}"/>
-    <hyperlink ref="R2" r:id="rId5" xr:uid="{4FFAFDCD-4BE1-4BCE-80AB-2E37BBABAB9A}"/>
-    <hyperlink ref="N2" r:id="rId6" xr:uid="{98118376-DAD7-4723-9647-1238A799648D}"/>
-    <hyperlink ref="J2" r:id="rId7" xr:uid="{4D13065F-02BC-4E8C-8A59-DB44B3A09884}"/>
-    <hyperlink ref="P2" r:id="rId8" xr:uid="{E3DAF414-5CC4-4981-A936-2B07B93582E5}"/>
-    <hyperlink ref="O2" r:id="rId9" xr:uid="{29B76FC0-060F-4028-BC19-EEB29C21C3D6}"/>
+    <hyperlink ref="K23" r:id="rId1" xr:uid="{7507FAC6-3C31-4D34-96D3-809B037A1804}"/>
+    <hyperlink ref="L23" r:id="rId2" xr:uid="{4B2682E2-45B8-4BB8-ACD2-5E05F6C13CF9}"/>
+    <hyperlink ref="M23" r:id="rId3" xr:uid="{B4188B97-9CCE-4810-A77D-E94661EB9F84}"/>
+    <hyperlink ref="Q23" r:id="rId4" xr:uid="{1E7D945F-FEE7-4F42-9704-096D37B64E27}"/>
+    <hyperlink ref="R23" r:id="rId5" xr:uid="{4FFAFDCD-4BE1-4BCE-80AB-2E37BBABAB9A}"/>
+    <hyperlink ref="N23" r:id="rId6" xr:uid="{98118376-DAD7-4723-9647-1238A799648D}"/>
+    <hyperlink ref="J23" r:id="rId7" xr:uid="{4D13065F-02BC-4E8C-8A59-DB44B3A09884}"/>
+    <hyperlink ref="P23" r:id="rId8" xr:uid="{E3DAF414-5CC4-4981-A936-2B07B93582E5}"/>
+    <hyperlink ref="O23" r:id="rId9" xr:uid="{29B76FC0-060F-4028-BC19-EEB29C21C3D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>